<commit_message>
P10 / Sprint 04
</commit_message>
<xml_diff>
--- a/P10/docs/Scrum.xlsx
+++ b/P10/docs/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kolade Favour\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F13A605-D12D-41D1-9408-BE5A6B03797D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D08002-BA41-45BF-9F23-E6C60C2EAD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="214">
   <si>
     <t>Product Name:</t>
   </si>
@@ -804,6 +804,27 @@
   </si>
   <si>
     <t>create buttons and add to the toolbar for rabbit</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 4</t>
+  </si>
+  <si>
+    <t>create generic for animal types</t>
+  </si>
+  <si>
+    <t>list all clients in the adoption centre</t>
+  </si>
+  <si>
+    <t>write create method for animals to use in generic</t>
+  </si>
+  <si>
+    <t>override create method for animals to use in generic</t>
+  </si>
+  <si>
+    <t>make button for client</t>
+  </si>
+  <si>
+    <t>make button for other animal</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1345,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2550,22 +2571,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3628,8 +3649,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView topLeftCell="A38" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -3909,11 +3930,11 @@
       </c>
       <c r="B16" s="2">
         <f>B15-C16</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$104,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="2"/>
@@ -3929,11 +3950,11 @@
       </c>
       <c r="B17" s="2">
         <f>B16-C17</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$104,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="2"/>
@@ -4589,7 +4610,9 @@
       <c r="F40" s="16">
         <v>4</v>
       </c>
-      <c r="G40" s="16"/>
+      <c r="G40" s="16" t="s">
+        <v>203</v>
+      </c>
       <c r="H40" s="22" t="s">
         <v>36</v>
       </c>
@@ -6674,7 +6697,7 @@
         <v>4</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H42" s="22" t="s">
         <v>36</v>
@@ -6706,7 +6729,9 @@
       <c r="F43" s="16">
         <v>4</v>
       </c>
-      <c r="G43" s="16"/>
+      <c r="G43" s="16" t="s">
+        <v>207</v>
+      </c>
       <c r="H43" s="22" t="s">
         <v>108</v>
       </c>
@@ -6822,7 +6847,7 @@
       </c>
       <c r="F48" s="16"/>
       <c r="G48" s="16" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H48" s="22" t="s">
         <v>108</v>
@@ -10833,8 +10858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -10938,7 +10963,7 @@
       </c>
       <c r="B7" s="31">
         <f>COUNTA(D17:D995)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
@@ -10953,7 +10978,7 @@
       </c>
       <c r="B8" s="31">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C8" s="31">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -10971,7 +10996,7 @@
       </c>
       <c r="B9" s="31">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C9" s="31">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -10989,7 +11014,7 @@
       </c>
       <c r="B10" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C10" s="31">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -11007,7 +11032,7 @@
       </c>
       <c r="B11" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C11" s="31">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -11025,11 +11050,11 @@
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C12" s="31">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
@@ -11047,7 +11072,7 @@
       </c>
       <c r="C13" s="31">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
@@ -11128,7 +11153,7 @@
         <v>202</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11177,57 +11202,99 @@
       <c r="A22">
         <v>6</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="41"/>
+      <c r="B22" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
         <v>7</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="41"/>
+      <c r="B23" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
         <v>8</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="41"/>
+      <c r="B24" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
         <v>9</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="41"/>
+      <c r="B25" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
         <v>10</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="41"/>
+      <c r="B26" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
         <v>11</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="41"/>
+      <c r="B27" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
         <v>12</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="41"/>
+      <c r="B28" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">

</xml_diff>